<commit_message>
Initial spreadsheet, needs openstudio-standards gem on server
</commit_message>
<xml_diff>
--- a/spreadsheet/template.xlsx
+++ b/spreadsheet/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="23256" windowHeight="13116" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2402" uniqueCount="815">
   <si>
     <t>type</t>
   </si>
@@ -2130,9 +2130,6 @@
     <t>../measures</t>
   </si>
   <si>
-    <t>../weather/USA_CO_Denver.Intl.AP.725650_TMY3.epw</t>
-  </si>
-  <si>
     <t>Can be used as worker</t>
   </si>
   <si>
@@ -2277,9 +2274,6 @@
     <t>empty seed</t>
   </si>
   <si>
-    <t>../seeds/empty.osm</t>
-  </si>
-  <si>
     <t>ChangeBuildingLocation</t>
   </si>
   <si>
@@ -2361,9 +2355,6 @@
     <t>__SKIP__</t>
   </si>
   <si>
-    <t>[0,1]</t>
-  </si>
-  <si>
     <t>[0.5,0.5]</t>
   </si>
   <si>
@@ -2416,6 +2407,84 @@
   </si>
   <si>
     <t>Set Motor Efficiency (%)</t>
+  </si>
+  <si>
+    <t>Skip 1</t>
+  </si>
+  <si>
+    <t>Skip 2</t>
+  </si>
+  <si>
+    <t>Skip 3</t>
+  </si>
+  <si>
+    <t>Skip 4</t>
+  </si>
+  <si>
+    <t>Skip 5</t>
+  </si>
+  <si>
+    <t>Skip 6</t>
+  </si>
+  <si>
+    <t>Seeds</t>
+  </si>
+  <si>
+    <t>../seed/empty.osm</t>
+  </si>
+  <si>
+    <t>../seed/</t>
+  </si>
+  <si>
+    <t>seed</t>
+  </si>
+  <si>
+    <t>../weather/*.*</t>
+  </si>
+  <si>
+    <t>[2, 3, 4]</t>
+  </si>
+  <si>
+    <t>[0.33,0.34,0.33]</t>
+  </si>
+  <si>
+    <t>[TRUE, FALSE]</t>
+  </si>
+  <si>
+    <t>urban_building_type</t>
+  </si>
+  <si>
+    <t>UrbanBuildingType</t>
+  </si>
+  <si>
+    <t>Urban Building Type</t>
+  </si>
+  <si>
+    <t>heating_source</t>
+  </si>
+  <si>
+    <t>cooling_source</t>
+  </si>
+  <si>
+    <t>Cooling source</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>[0.25, 0.25, 0.25, 0.25]</t>
+  </si>
+  <si>
+    <t>["Electric", "District Chilled Water", "District Ambient Water"]</t>
+  </si>
+  <si>
+    <t>["Gas", "Electric", "District Hot Water", "District Ambient Water"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heating source </t>
   </si>
 </sst>
 </file>
@@ -4109,7 +4178,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4223,6 +4292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6029,7 +6099,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6067,7 +6137,7 @@
         <v>435</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>436</v>
@@ -6078,7 +6148,7 @@
         <v>457</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>458</v>
@@ -6089,7 +6159,7 @@
         <v>470</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>611</v>
@@ -6100,7 +6170,7 @@
         <v>471</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>473</v>
@@ -6168,21 +6238,21 @@
         <v>$0.28/hour</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
+        <v>698</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>699</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>700</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6200,7 +6270,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>472</v>
@@ -6247,7 +6317,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -6291,7 +6361,7 @@
         <v>452</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>15</v>
+        <v>711</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
@@ -6320,15 +6390,15 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$30,0)-2))=0,"",INDEX(Lookups!$C$19:$AI$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$30,0)-2))</f>
-        <v>Sample Method</v>
+        <v/>
       </c>
       <c r="B25" s="18" t="str">
         <f>IF(D25&lt;&gt;"",D25,IF(LEN(INDEX(Lookups!$C$19:$AI$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$30,0)-1))=0,"",INDEX(Lookups!$C$19:$AI$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$30,0)-1)))</f>
-        <v>individual_variables</v>
+        <v/>
       </c>
       <c r="C25" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$29,0)))</f>
-        <v>individual_variables / all_variables</v>
+        <v/>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="23"/>
@@ -6336,7 +6406,7 @@
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="23" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$30,0)-2))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$30,0)-2))</f>
-        <v>Number of Samples</v>
+        <v/>
       </c>
       <c r="B26" s="18">
         <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$30,0)-1))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$30,0)-1)))</f>
@@ -6344,7 +6414,7 @@
       </c>
       <c r="C26" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$29,0)))</f>
-        <v>positive integer (if individual, total simulations is this times each variable)</v>
+        <v/>
       </c>
       <c r="D26" s="27">
         <v>40</v>
@@ -6550,12 +6620,12 @@
       <c r="E39" s="6"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>696</v>
+        <v>799</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6581,13 +6651,13 @@
         <v>31</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>745</v>
+        <v>796</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>449</v>
@@ -6609,20 +6679,31 @@
         <v>610</v>
       </c>
     </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="55" t="s">
+        <v>795</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>798</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>797</v>
+      </c>
+    </row>
     <row r="48" spans="1:6" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
+        <v>701</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>702</v>
       </c>
-      <c r="B48" s="19" t="s">
+      <c r="C48" s="6" t="s">
         <v>703</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>704</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="19"/>
       <c r="F48" s="8" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -6637,18 +6718,18 @@
     </row>
     <row r="51" spans="1:6" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
+        <v>705</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>706</v>
       </c>
-      <c r="B51" s="19" t="s">
-        <v>707</v>
-      </c>
       <c r="C51" s="6" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="19"/>
       <c r="F51" s="8" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
   </sheetData>
@@ -6682,10 +6763,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z71"/>
+  <dimension ref="A1:Z74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6869,13 +6950,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>67</v>
@@ -6909,10 +6990,10 @@
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15" t="s">
@@ -6920,7 +7001,7 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -6945,16 +7026,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>103</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
@@ -7002,10 +7083,10 @@
       </c>
       <c r="C8" s="35"/>
       <c r="D8" s="35" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="F8" s="35"/>
       <c r="G8" s="35" t="s">
@@ -7022,13 +7103,18 @@
       <c r="L8" s="35">
         <v>50000</v>
       </c>
-      <c r="M8" s="35"/>
-      <c r="N8" s="36"/>
+      <c r="M8" s="35">
+        <f>(L8+K8)/2</f>
+        <v>27500</v>
+      </c>
+      <c r="N8" s="36">
+        <v>1</v>
+      </c>
       <c r="O8" s="36"/>
       <c r="P8" s="36"/>
       <c r="Q8" s="36"/>
       <c r="R8" s="35" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="S8" s="35"/>
       <c r="T8" s="35"/>
@@ -7046,7 +7132,7 @@
       </c>
       <c r="C9" s="35"/>
       <c r="D9" s="35" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E9" s="35" t="s">
         <v>199</v>
@@ -7066,13 +7152,18 @@
       <c r="L9" s="35">
         <v>4</v>
       </c>
-      <c r="M9" s="35"/>
-      <c r="N9" s="36"/>
+      <c r="M9" s="35">
+        <f t="shared" ref="M9:M11" si="0">(L9+K9)/2</f>
+        <v>2.125</v>
+      </c>
+      <c r="N9" s="36">
+        <v>1</v>
+      </c>
       <c r="O9" s="36"/>
       <c r="P9" s="36"/>
       <c r="Q9" s="36"/>
       <c r="R9" s="35" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="S9" s="35"/>
       <c r="T9" s="35"/>
@@ -7090,10 +7181,10 @@
       </c>
       <c r="C10" s="35"/>
       <c r="D10" s="35" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="F10" s="35"/>
       <c r="G10" s="35" t="s">
@@ -7110,13 +7201,18 @@
       <c r="L10" s="35">
         <v>0.8</v>
       </c>
-      <c r="M10" s="35"/>
-      <c r="N10" s="36"/>
+      <c r="M10" s="35">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N10" s="36">
+        <v>1</v>
+      </c>
       <c r="O10" s="36"/>
       <c r="P10" s="36"/>
       <c r="Q10" s="36"/>
       <c r="R10" s="35" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="S10" s="35"/>
       <c r="T10" s="35"/>
@@ -7134,14 +7230,14 @@
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="35" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F11" s="35"/>
       <c r="G11" s="35" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H11" s="35"/>
       <c r="I11" s="35">
@@ -7154,13 +7250,22 @@
       <c r="L11" s="35">
         <v>4</v>
       </c>
-      <c r="M11" s="35"/>
-      <c r="N11" s="36"/>
+      <c r="M11" s="35">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N11" s="36">
+        <v>1</v>
+      </c>
       <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
+      <c r="P11" s="36" t="s">
+        <v>800</v>
+      </c>
+      <c r="Q11" s="36" t="s">
+        <v>801</v>
+      </c>
       <c r="R11" s="35" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="S11" s="35"/>
       <c r="T11" s="35"/>
@@ -7176,10 +7281,10 @@
         <v>21</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>63</v>
@@ -7193,13 +7298,13 @@
         <v>21</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>205</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I13" s="15" t="b">
         <v>1</v>
@@ -7210,13 +7315,13 @@
         <v>21</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>207</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I14" s="15" t="b">
         <v>1</v>
@@ -7227,13 +7332,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E15" s="32" t="s">
         <v>67</v>
@@ -7265,7 +7370,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>44</v>
@@ -7274,7 +7379,7 @@
         <v>103</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
     </row>
     <row r="17" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
@@ -7284,14 +7389,14 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15">
@@ -7315,18 +7420,18 @@
       <c r="Y17" s="15"/>
       <c r="Z17" s="15"/>
     </row>
-    <row r="18" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="b">
         <v>1</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>284</v>
+        <v>805</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>285</v>
+        <v>803</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>285</v>
+        <v>804</v>
       </c>
       <c r="E18" s="32" t="s">
         <v>67</v>
@@ -7360,33 +7465,43 @@
       </c>
       <c r="C19" s="35"/>
       <c r="D19" s="35" t="s">
-        <v>771</v>
+        <v>814</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>772</v>
+        <v>806</v>
       </c>
       <c r="F19" s="35"/>
       <c r="G19" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H19" s="35"/>
-      <c r="I19" s="35">
-        <v>0</v>
-      </c>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
+      <c r="I19" s="35" t="s">
+        <v>809</v>
+      </c>
+      <c r="J19" s="35" t="s">
+        <v>813</v>
+      </c>
+      <c r="K19" s="35" t="s">
+        <v>809</v>
+      </c>
+      <c r="L19" s="35" t="s">
+        <v>809</v>
+      </c>
+      <c r="M19" s="35" t="s">
+        <v>809</v>
+      </c>
+      <c r="N19" s="35" t="s">
+        <v>809</v>
+      </c>
+      <c r="O19" s="36"/>
       <c r="P19" s="35" t="s">
-        <v>773</v>
-      </c>
-      <c r="Q19" s="35" t="s">
-        <v>774</v>
+        <v>813</v>
+      </c>
+      <c r="Q19" s="36" t="s">
+        <v>811</v>
       </c>
       <c r="R19" s="35" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="S19" s="35"/>
       <c r="T19" s="35"/>
@@ -7397,812 +7512,920 @@
       <c r="Y19" s="35"/>
       <c r="Z19" s="35"/>
     </row>
-    <row r="20" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>768</v>
-      </c>
-      <c r="E20" s="15" t="s">
+    <row r="20" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35" t="s">
+        <v>808</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>807</v>
+      </c>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35" t="s">
+        <v>810</v>
+      </c>
+      <c r="J20" s="35" t="s">
+        <v>812</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>810</v>
+      </c>
+      <c r="L20" s="35" t="s">
+        <v>810</v>
+      </c>
+      <c r="M20" s="35" t="s">
+        <v>810</v>
+      </c>
+      <c r="N20" s="35" t="s">
+        <v>810</v>
+      </c>
+      <c r="O20" s="36"/>
+      <c r="P20" s="35" t="s">
+        <v>812</v>
+      </c>
+      <c r="Q20" s="36" t="s">
+        <v>801</v>
+      </c>
+      <c r="R20" s="35" t="s">
+        <v>735</v>
+      </c>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
+      <c r="X20" s="35"/>
+      <c r="Y20" s="35"/>
+      <c r="Z20" s="35"/>
+    </row>
+    <row r="21" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="32"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="32"/>
+      <c r="Z21" s="32"/>
+    </row>
+    <row r="22" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="35"/>
+      <c r="B22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35" t="s">
+        <v>769</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>770</v>
+      </c>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35" t="s">
+        <v>763</v>
+      </c>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35" t="s">
+        <v>802</v>
+      </c>
+      <c r="Q22" s="35" t="s">
+        <v>771</v>
+      </c>
+      <c r="R22" s="35" t="s">
+        <v>735</v>
+      </c>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="35"/>
+      <c r="Z22" s="35"/>
+    </row>
+    <row r="23" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>766</v>
+      </c>
+      <c r="E23" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G23" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="I23" s="15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="15" t="s">
+    <row r="24" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>775</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>772</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>772</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>772</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="32"/>
+      <c r="Y25" s="32"/>
+      <c r="Z25" s="32"/>
+    </row>
+    <row r="26" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="35"/>
+      <c r="B26" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35" t="s">
+        <v>789</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>770</v>
+      </c>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35" t="s">
+        <v>763</v>
+      </c>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M26" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="N26" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O26" s="35"/>
+      <c r="P26" s="35" t="s">
+        <v>802</v>
+      </c>
+      <c r="Q26" s="35" t="s">
+        <v>771</v>
+      </c>
+      <c r="R26" s="35" t="s">
+        <v>735</v>
+      </c>
+      <c r="S26" s="35"/>
+      <c r="T26" s="35"/>
+      <c r="U26" s="35"/>
+      <c r="V26" s="35"/>
+      <c r="W26" s="35"/>
+      <c r="X26" s="35"/>
+      <c r="Y26" s="35"/>
+      <c r="Z26" s="35"/>
+    </row>
+    <row r="27" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="32"/>
+      <c r="V27" s="32"/>
+      <c r="W27" s="32"/>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="32"/>
+    </row>
+    <row r="28" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="35"/>
+      <c r="B28" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35" t="s">
+        <v>790</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>770</v>
+      </c>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35" t="s">
+        <v>763</v>
+      </c>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M28" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="N28" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O28" s="35"/>
+      <c r="P28" s="35" t="s">
+        <v>802</v>
+      </c>
+      <c r="Q28" s="35" t="s">
+        <v>771</v>
+      </c>
+      <c r="R28" s="35" t="s">
+        <v>735</v>
+      </c>
+      <c r="S28" s="35"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="35"/>
+      <c r="V28" s="35"/>
+      <c r="W28" s="35"/>
+      <c r="X28" s="35"/>
+      <c r="Y28" s="35"/>
+      <c r="Z28" s="35"/>
+    </row>
+    <row r="29" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>766</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>776</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>773</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>773</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>773</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="32"/>
+      <c r="T31" s="32"/>
+      <c r="U31" s="32"/>
+      <c r="V31" s="32"/>
+      <c r="W31" s="32"/>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="32"/>
+      <c r="Z31" s="32"/>
+    </row>
+    <row r="32" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="35"/>
+      <c r="B32" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35" t="s">
+        <v>791</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>770</v>
+      </c>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35" t="s">
+        <v>763</v>
+      </c>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L32" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M32" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="N32" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O32" s="35"/>
+      <c r="P32" s="35" t="s">
+        <v>802</v>
+      </c>
+      <c r="Q32" s="35" t="s">
+        <v>771</v>
+      </c>
+      <c r="R32" s="35" t="s">
+        <v>735</v>
+      </c>
+      <c r="S32" s="35"/>
+      <c r="T32" s="35"/>
+      <c r="U32" s="35"/>
+      <c r="V32" s="35"/>
+      <c r="W32" s="35"/>
+      <c r="X32" s="35"/>
+      <c r="Y32" s="35"/>
+      <c r="Z32" s="35"/>
+    </row>
+    <row r="33" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>774</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>774</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>774</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
+      <c r="W33" s="32"/>
+      <c r="X33" s="32"/>
+      <c r="Y33" s="32"/>
+      <c r="Z33" s="32"/>
+    </row>
+    <row r="34" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="35"/>
+      <c r="B34" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35" t="s">
+        <v>792</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>770</v>
+      </c>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35" t="s">
+        <v>763</v>
+      </c>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L34" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M34" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="N34" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O34" s="35"/>
+      <c r="P34" s="35" t="s">
+        <v>802</v>
+      </c>
+      <c r="Q34" s="35" t="s">
+        <v>771</v>
+      </c>
+      <c r="R34" s="35" t="s">
+        <v>735</v>
+      </c>
+      <c r="S34" s="35"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="35"/>
+      <c r="V34" s="35"/>
+      <c r="W34" s="35"/>
+      <c r="X34" s="35"/>
+      <c r="Y34" s="35"/>
+      <c r="Z34" s="35"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A35" s="15"/>
+      <c r="B35" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>777</v>
+      </c>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="15"/>
+      <c r="V35" s="15"/>
+      <c r="W35" s="15"/>
+      <c r="X35" s="15"/>
+      <c r="Y35" s="15"/>
+      <c r="Z35" s="15"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A36" s="15"/>
+      <c r="B36" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15" t="s">
+        <v>779</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>778</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="G21" s="15" t="s">
+      <c r="F36" s="15"/>
+      <c r="G36" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I21" s="15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="32" t="b">
+      <c r="H36" s="15"/>
+      <c r="I36" s="15">
+        <v>1.3</v>
+      </c>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="15"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="15"/>
+      <c r="X36" s="15"/>
+      <c r="Y36" s="15"/>
+      <c r="Z36" s="15"/>
+    </row>
+    <row r="37" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="32" t="b">
         <v>1</v>
       </c>
-      <c r="B22" s="32" t="s">
-        <v>775</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>775</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>775</v>
-      </c>
-      <c r="E22" s="32" t="s">
+      <c r="B37" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="E37" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="32"/>
-      <c r="R22" s="32"/>
-      <c r="S22" s="32"/>
-      <c r="T22" s="32"/>
-      <c r="U22" s="32"/>
-      <c r="V22" s="32"/>
-      <c r="W22" s="32"/>
-      <c r="X22" s="32"/>
-      <c r="Y22" s="32"/>
-      <c r="Z22" s="32"/>
-    </row>
-    <row r="23" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35" t="s">
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="32"/>
+      <c r="L37" s="32"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="32"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
+      <c r="W37" s="32"/>
+      <c r="X37" s="32"/>
+      <c r="Y37" s="32"/>
+      <c r="Z37" s="32"/>
+    </row>
+    <row r="38" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="35"/>
+      <c r="B38" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35" t="s">
+      <c r="C38" s="35"/>
+      <c r="D38" s="35" t="s">
+        <v>793</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>770</v>
+      </c>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35" t="s">
+        <v>763</v>
+      </c>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L38" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M38" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="N38" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O38" s="35"/>
+      <c r="P38" s="35" t="s">
+        <v>802</v>
+      </c>
+      <c r="Q38" s="35" t="s">
         <v>771</v>
       </c>
-      <c r="E23" s="35" t="s">
-        <v>772</v>
-      </c>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35">
-        <v>0</v>
-      </c>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35" t="s">
-        <v>773</v>
-      </c>
-      <c r="Q23" s="35" t="s">
-        <v>774</v>
-      </c>
-      <c r="R23" s="35" t="s">
-        <v>736</v>
-      </c>
-      <c r="S23" s="35"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
-      <c r="X23" s="35"/>
-      <c r="Y23" s="35"/>
-      <c r="Z23" s="35"/>
-    </row>
-    <row r="24" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="32"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="32"/>
-      <c r="V24" s="32"/>
-      <c r="W24" s="32"/>
-      <c r="X24" s="32"/>
-      <c r="Y24" s="32"/>
-      <c r="Z24" s="32"/>
-    </row>
-    <row r="25" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
-      <c r="B25" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35" t="s">
-        <v>771</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>772</v>
-      </c>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35">
-        <v>0</v>
-      </c>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35" t="s">
-        <v>773</v>
-      </c>
-      <c r="Q25" s="35" t="s">
-        <v>774</v>
-      </c>
-      <c r="R25" s="35" t="s">
-        <v>736</v>
-      </c>
-      <c r="S25" s="35"/>
-      <c r="T25" s="35"/>
-      <c r="U25" s="35"/>
-      <c r="V25" s="35"/>
-      <c r="W25" s="35"/>
-      <c r="X25" s="35"/>
-      <c r="Y25" s="35"/>
-      <c r="Z25" s="35"/>
-    </row>
-    <row r="26" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>768</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="15" t="s">
+      <c r="R38" s="35" t="s">
+        <v>735</v>
+      </c>
+      <c r="S38" s="35"/>
+      <c r="T38" s="35"/>
+      <c r="U38" s="35"/>
+      <c r="V38" s="35"/>
+      <c r="W38" s="35"/>
+      <c r="X38" s="35"/>
+      <c r="Y38" s="35"/>
+      <c r="Z38" s="35"/>
+    </row>
+    <row r="39" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>781</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G39" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="I26" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>779</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" s="15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="B28" s="32" t="s">
-        <v>776</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>776</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>776</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="32"/>
-      <c r="N28" s="32"/>
-      <c r="O28" s="32"/>
-      <c r="P28" s="32"/>
-      <c r="Q28" s="32"/>
-      <c r="R28" s="32"/>
-      <c r="S28" s="32"/>
-      <c r="T28" s="32"/>
-      <c r="U28" s="32"/>
-      <c r="V28" s="32"/>
-      <c r="W28" s="32"/>
-      <c r="X28" s="32"/>
-      <c r="Y28" s="32"/>
-      <c r="Z28" s="32"/>
-    </row>
-    <row r="29" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
-      <c r="B29" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35" t="s">
-        <v>771</v>
-      </c>
-      <c r="E29" s="35" t="s">
-        <v>772</v>
-      </c>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35">
-        <v>0</v>
-      </c>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="35" t="s">
-        <v>773</v>
-      </c>
-      <c r="Q29" s="35" t="s">
-        <v>774</v>
-      </c>
-      <c r="R29" s="35" t="s">
-        <v>736</v>
-      </c>
-      <c r="S29" s="35"/>
-      <c r="T29" s="35"/>
-      <c r="U29" s="35"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="35"/>
-      <c r="X29" s="35"/>
-      <c r="Y29" s="35"/>
-      <c r="Z29" s="35"/>
-    </row>
-    <row r="30" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>777</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>777</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>777</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="32"/>
-      <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="32"/>
-      <c r="R30" s="32"/>
-      <c r="S30" s="32"/>
-      <c r="T30" s="32"/>
-      <c r="U30" s="32"/>
-      <c r="V30" s="32"/>
-      <c r="W30" s="32"/>
-      <c r="X30" s="32"/>
-      <c r="Y30" s="32"/>
-      <c r="Z30" s="32"/>
-    </row>
-    <row r="31" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
-      <c r="B31" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35" t="s">
-        <v>771</v>
-      </c>
-      <c r="E31" s="35" t="s">
-        <v>772</v>
-      </c>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35">
-        <v>0</v>
-      </c>
-      <c r="J31" s="35"/>
-      <c r="K31" s="35"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
-      <c r="O31" s="35"/>
-      <c r="P31" s="35" t="s">
-        <v>773</v>
-      </c>
-      <c r="Q31" s="35" t="s">
-        <v>774</v>
-      </c>
-      <c r="R31" s="35" t="s">
-        <v>736</v>
-      </c>
-      <c r="S31" s="35"/>
-      <c r="T31" s="35"/>
-      <c r="U31" s="35"/>
-      <c r="V31" s="35"/>
-      <c r="W31" s="35"/>
-      <c r="X31" s="35"/>
-      <c r="Y31" s="35"/>
-      <c r="Z31" s="35"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15" t="s">
-        <v>783</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>780</v>
-      </c>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
-      <c r="T32" s="15"/>
-      <c r="U32" s="15"/>
-      <c r="V32" s="15"/>
-      <c r="W32" s="15"/>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="15"/>
-      <c r="Z32" s="15"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15" t="s">
-        <v>782</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>781</v>
-      </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15">
-        <v>1.3</v>
-      </c>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
-      <c r="T33" s="15"/>
-      <c r="U33" s="15"/>
-      <c r="V33" s="15"/>
-      <c r="W33" s="15"/>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="15"/>
-      <c r="Z33" s="15"/>
-    </row>
-    <row r="34" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="B34" s="32" t="s">
-        <v>241</v>
-      </c>
-      <c r="C34" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="D34" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="E34" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
-      <c r="P34" s="32"/>
-      <c r="Q34" s="32"/>
-      <c r="R34" s="32"/>
-      <c r="S34" s="32"/>
-      <c r="T34" s="32"/>
-      <c r="U34" s="32"/>
-      <c r="V34" s="32"/>
-      <c r="W34" s="32"/>
-      <c r="X34" s="32"/>
-      <c r="Y34" s="32"/>
-      <c r="Z34" s="32"/>
-    </row>
-    <row r="35" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="35"/>
-      <c r="B35" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35" t="s">
-        <v>771</v>
-      </c>
-      <c r="E35" s="35" t="s">
-        <v>772</v>
-      </c>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35">
-        <v>0</v>
-      </c>
-      <c r="J35" s="35"/>
-      <c r="K35" s="35"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="35"/>
-      <c r="O35" s="35"/>
-      <c r="P35" s="35" t="s">
-        <v>773</v>
-      </c>
-      <c r="Q35" s="35" t="s">
-        <v>774</v>
-      </c>
-      <c r="R35" s="35" t="s">
-        <v>736</v>
-      </c>
-      <c r="S35" s="35"/>
-      <c r="T35" s="35"/>
-      <c r="U35" s="35"/>
-      <c r="V35" s="35"/>
-      <c r="W35" s="35"/>
-      <c r="X35" s="35"/>
-      <c r="Y35" s="35"/>
-      <c r="Z35" s="35"/>
-    </row>
-    <row r="36" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>784</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="I36" s="15" t="s">
+      <c r="I39" s="15" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>785</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I37" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>786</v>
-      </c>
-      <c r="C38" s="32" t="s">
-        <v>250</v>
-      </c>
-      <c r="D38" s="32" t="s">
-        <v>250</v>
-      </c>
-      <c r="E38" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="32"/>
-      <c r="R38" s="32"/>
-      <c r="S38" s="32"/>
-      <c r="T38" s="32"/>
-      <c r="U38" s="32"/>
-      <c r="V38" s="32"/>
-      <c r="W38" s="32"/>
-      <c r="X38" s="32"/>
-      <c r="Y38" s="32"/>
-      <c r="Z38" s="32"/>
-    </row>
-    <row r="39" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35" t="s">
-        <v>771</v>
-      </c>
-      <c r="E39" s="35" t="s">
-        <v>772</v>
-      </c>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="H39" s="35"/>
-      <c r="I39" s="35">
-        <v>0</v>
-      </c>
-      <c r="J39" s="35"/>
-      <c r="K39" s="35"/>
-      <c r="L39" s="35"/>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="P39" s="35" t="s">
-        <v>773</v>
-      </c>
-      <c r="Q39" s="35" t="s">
-        <v>774</v>
-      </c>
-      <c r="R39" s="35" t="s">
-        <v>736</v>
-      </c>
-      <c r="S39" s="35"/>
-      <c r="T39" s="35"/>
-      <c r="U39" s="35"/>
-      <c r="V39" s="35"/>
-      <c r="W39" s="35"/>
-      <c r="X39" s="35"/>
-      <c r="Y39" s="35"/>
-      <c r="Z39" s="35"/>
     </row>
     <row r="40" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
       <c r="E40" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I40" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>783</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="32"/>
+      <c r="U41" s="32"/>
+      <c r="V41" s="32"/>
+      <c r="W41" s="32"/>
+      <c r="X41" s="32"/>
+      <c r="Y41" s="32"/>
+      <c r="Z41" s="32"/>
+    </row>
+    <row r="42" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="35"/>
+      <c r="B42" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35" t="s">
+        <v>794</v>
+      </c>
+      <c r="E42" s="35" t="s">
+        <v>770</v>
+      </c>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35" t="s">
+        <v>763</v>
+      </c>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L42" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M42" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="N42" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O42" s="35"/>
+      <c r="P42" s="35" t="s">
+        <v>802</v>
+      </c>
+      <c r="Q42" s="35" t="s">
+        <v>771</v>
+      </c>
+      <c r="R42" s="35" t="s">
+        <v>735</v>
+      </c>
+      <c r="S42" s="35"/>
+      <c r="T42" s="35"/>
+      <c r="U42" s="35"/>
+      <c r="V42" s="35"/>
+      <c r="W42" s="35"/>
+      <c r="X42" s="35"/>
+      <c r="Y42" s="35"/>
+      <c r="Z42" s="35"/>
+    </row>
+    <row r="43" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>784</v>
+      </c>
+      <c r="E43" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="G43" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="I40" s="15" t="s">
+      <c r="I43" s="15" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="41" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>791</v>
-      </c>
-      <c r="E41" s="15" t="s">
+    <row r="44" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>788</v>
+      </c>
+      <c r="E44" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="G41" s="15" t="s">
+      <c r="G44" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I41" s="15">
+      <c r="I44" s="15">
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="53" t="b">
+    <row r="45" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="B42" s="53" t="s">
-        <v>788</v>
-      </c>
-      <c r="C42" s="53" t="s">
-        <v>789</v>
-      </c>
-      <c r="D42" s="53" t="s">
-        <v>789</v>
-      </c>
-      <c r="E42" s="53" t="s">
+      <c r="B45" s="53" t="s">
+        <v>785</v>
+      </c>
+      <c r="C45" s="53" t="s">
+        <v>786</v>
+      </c>
+      <c r="D45" s="53" t="s">
+        <v>786</v>
+      </c>
+      <c r="E45" s="53" t="s">
         <v>232</v>
       </c>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
-      <c r="U43" s="15"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="15"/>
-      <c r="X43" s="15"/>
-      <c r="Y43" s="15"/>
-      <c r="Z43" s="15"/>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
-      <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="15"/>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A45" s="15"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15"/>
-      <c r="R45" s="15"/>
-      <c r="S45" s="15"/>
-      <c r="T45" s="15"/>
-      <c r="U45" s="15"/>
-      <c r="V45" s="15"/>
-      <c r="W45" s="15"/>
-      <c r="X45" s="15"/>
-      <c r="Y45" s="15"/>
-      <c r="Z45" s="15"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="15"/>
@@ -8219,8 +8442,8 @@
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
-      <c r="O46" s="34"/>
-      <c r="P46" s="34"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
       <c r="S46" s="15"/>
@@ -8303,8 +8526,8 @@
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
       <c r="N49" s="15"/>
-      <c r="O49" s="15"/>
-      <c r="P49" s="15"/>
+      <c r="O49" s="34"/>
+      <c r="P49" s="34"/>
       <c r="Q49" s="15"/>
       <c r="R49" s="15"/>
       <c r="S49" s="15"/>
@@ -8387,8 +8610,8 @@
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
-      <c r="O52" s="34"/>
-      <c r="P52" s="34"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
       <c r="S52" s="15"/>
@@ -8471,8 +8694,8 @@
       <c r="L55" s="15"/>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
+      <c r="O55" s="34"/>
+      <c r="P55" s="34"/>
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
       <c r="S55" s="15"/>
@@ -8583,8 +8806,8 @@
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
-      <c r="O59" s="34"/>
-      <c r="P59" s="34"/>
+      <c r="O59" s="15"/>
+      <c r="P59" s="15"/>
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
       <c r="S59" s="15"/>
@@ -8639,8 +8862,8 @@
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
       <c r="N61" s="15"/>
-      <c r="O61" s="34"/>
-      <c r="P61" s="34"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
       <c r="Q61" s="15"/>
       <c r="R61" s="15"/>
       <c r="S61" s="15"/>
@@ -8751,8 +8974,8 @@
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
       <c r="N65" s="15"/>
-      <c r="O65" s="15"/>
-      <c r="P65" s="15"/>
+      <c r="O65" s="34"/>
+      <c r="P65" s="34"/>
       <c r="Q65" s="15"/>
       <c r="R65" s="15"/>
       <c r="S65" s="15"/>
@@ -8779,8 +9002,8 @@
       <c r="L66" s="15"/>
       <c r="M66" s="15"/>
       <c r="N66" s="15"/>
-      <c r="O66" s="34"/>
-      <c r="P66" s="34"/>
+      <c r="O66" s="15"/>
+      <c r="P66" s="15"/>
       <c r="Q66" s="15"/>
       <c r="R66" s="15"/>
       <c r="S66" s="15"/>
@@ -8807,8 +9030,8 @@
       <c r="L67" s="15"/>
       <c r="M67" s="15"/>
       <c r="N67" s="15"/>
-      <c r="O67" s="15"/>
-      <c r="P67" s="15"/>
+      <c r="O67" s="34"/>
+      <c r="P67" s="34"/>
       <c r="Q67" s="15"/>
       <c r="R67" s="15"/>
       <c r="S67" s="15"/>
@@ -8835,8 +9058,8 @@
       <c r="L68" s="15"/>
       <c r="M68" s="15"/>
       <c r="N68" s="15"/>
-      <c r="O68" s="34"/>
-      <c r="P68" s="34"/>
+      <c r="O68" s="15"/>
+      <c r="P68" s="15"/>
       <c r="Q68" s="15"/>
       <c r="R68" s="15"/>
       <c r="S68" s="15"/>
@@ -8863,8 +9086,8 @@
       <c r="L69" s="15"/>
       <c r="M69" s="15"/>
       <c r="N69" s="15"/>
-      <c r="O69" s="15"/>
-      <c r="P69" s="15"/>
+      <c r="O69" s="34"/>
+      <c r="P69" s="34"/>
       <c r="Q69" s="15"/>
       <c r="R69" s="15"/>
       <c r="S69" s="15"/>
@@ -8891,8 +9114,8 @@
       <c r="L70" s="15"/>
       <c r="M70" s="15"/>
       <c r="N70" s="15"/>
-      <c r="O70" s="34"/>
-      <c r="P70" s="34"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="15"/>
       <c r="Q70" s="15"/>
       <c r="R70" s="15"/>
       <c r="S70" s="15"/>
@@ -8919,8 +9142,8 @@
       <c r="L71" s="15"/>
       <c r="M71" s="15"/>
       <c r="N71" s="15"/>
-      <c r="O71" s="15"/>
-      <c r="P71" s="15"/>
+      <c r="O71" s="34"/>
+      <c r="P71" s="34"/>
       <c r="Q71" s="15"/>
       <c r="R71" s="15"/>
       <c r="S71" s="15"/>
@@ -8931,6 +9154,90 @@
       <c r="X71" s="15"/>
       <c r="Y71" s="15"/>
       <c r="Z71" s="15"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A72" s="15"/>
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="O72" s="15"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
+      <c r="S72" s="15"/>
+      <c r="T72" s="15"/>
+      <c r="U72" s="15"/>
+      <c r="V72" s="15"/>
+      <c r="W72" s="15"/>
+      <c r="X72" s="15"/>
+      <c r="Y72" s="15"/>
+      <c r="Z72" s="15"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A73" s="15"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="34"/>
+      <c r="P73" s="34"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
+      <c r="S73" s="15"/>
+      <c r="T73" s="15"/>
+      <c r="U73" s="15"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="15"/>
+      <c r="X73" s="15"/>
+      <c r="Y73" s="15"/>
+      <c r="Z73" s="15"/>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A74" s="15"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="O74" s="15"/>
+      <c r="P74" s="15"/>
+      <c r="Q74" s="15"/>
+      <c r="R74" s="15"/>
+      <c r="S74" s="15"/>
+      <c r="T74" s="15"/>
+      <c r="U74" s="15"/>
+      <c r="V74" s="15"/>
+      <c r="W74" s="15"/>
+      <c r="X74" s="15"/>
+      <c r="Y74" s="15"/>
+      <c r="Z74" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -18246,7 +18553,7 @@
         <v>644</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -18263,7 +18570,7 @@
         <v>642</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -18280,7 +18587,7 @@
         <v>643</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -18297,7 +18604,7 @@
         <v>645</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -18314,7 +18621,7 @@
         <v>647</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -18367,7 +18674,7 @@
         <v>550</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
@@ -18387,18 +18694,18 @@
         <v>553</v>
       </c>
       <c r="X18" s="22" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="Y18" s="22"/>
       <c r="Z18" s="22"/>
       <c r="AA18" t="s">
+        <v>711</v>
+      </c>
+      <c r="AD18" t="s">
         <v>712</v>
       </c>
-      <c r="AD18" t="s">
-        <v>713</v>
-      </c>
       <c r="AG18" s="22" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AH18" s="22"/>
       <c r="AI18" s="22"/>
@@ -18408,13 +18715,13 @@
         <v>550</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G19" s="22">
         <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I19" t="s">
         <v>571</v>
@@ -18453,16 +18760,16 @@
         <v>580</v>
       </c>
       <c r="X19" s="22" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="Y19" s="22" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="Z19" s="22" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="AD19" s="22" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="AE19" s="22">
         <v>30</v>
@@ -18471,27 +18778,27 @@
         <v>589</v>
       </c>
       <c r="AG19" s="22" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="AH19" s="22" t="b">
         <v>1</v>
       </c>
       <c r="AI19" s="22" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G20" s="22">
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="I20" t="s">
         <v>4</v>
@@ -18536,16 +18843,16 @@
         <v>2</v>
       </c>
       <c r="Z20" s="22" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="AG20" s="22" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="AH20" s="22" t="b">
         <v>1</v>
       </c>
       <c r="AI20" s="22" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.3">
@@ -18553,7 +18860,7 @@
         <v>15</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="G21" s="22">
         <v>1</v>
@@ -18595,10 +18902,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>559</v>
@@ -18642,13 +18949,13 @@
         <v>541</v>
       </c>
       <c r="O23" s="22" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="P23" s="22">
         <v>1</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="R23" s="23" t="s">
         <v>568</v>
@@ -18703,13 +19010,13 @@
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="L25" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="M25" s="23">
+        <v>0</v>
+      </c>
+      <c r="N25" s="23" t="s">
         <v>715</v>
-      </c>
-      <c r="M25" s="23">
-        <v>0</v>
-      </c>
-      <c r="N25" s="23" t="s">
-        <v>716</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>539</v>
@@ -18721,18 +19028,18 @@
         <v>578</v>
       </c>
       <c r="R25" s="23" t="s">
+        <v>723</v>
+      </c>
+      <c r="S25" s="22">
+        <v>2</v>
+      </c>
+      <c r="T25" s="22" t="s">
         <v>724</v>
-      </c>
-      <c r="S25" s="22">
-        <v>2</v>
-      </c>
-      <c r="T25" s="22" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
@@ -18755,7 +19062,7 @@
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
@@ -18781,7 +19088,7 @@
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
@@ -18796,18 +19103,18 @@
         <v>575</v>
       </c>
       <c r="R28" t="s">
+        <v>714</v>
+      </c>
+      <c r="S28" s="23">
+        <v>0</v>
+      </c>
+      <c r="T28" s="23" t="s">
         <v>715</v>
-      </c>
-      <c r="S28" s="23">
-        <v>0</v>
-      </c>
-      <c r="T28" s="23" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
@@ -18838,13 +19145,13 @@
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
       <c r="O31" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="P31" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="23" t="s">
         <v>715</v>
-      </c>
-      <c r="P31" s="23">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="23" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
@@ -18852,13 +19159,13 @@
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
       <c r="O32" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="P32" s="23">
         <v>1</v>
       </c>
       <c r="Q32" s="23" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>